<commit_message>
añadido de notebook final
</commit_message>
<xml_diff>
--- a/otros/Borrador calculo angulo.xlsx
+++ b/otros/Borrador calculo angulo.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Consiltor2015\Documents\DIPLOMADO IA\CV\PUCP-VC-Grupo3-Volleyball\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Consiltor2015\Documents\DIPLOMADO IA\CV\PUCP-VC-Grupo3-Volleyball\otros\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F307EF50-B6D1-4F93-9C0C-47365CB469A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C3EC9FD-5AC1-4112-8A5F-FB63394C72EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{3763591E-8342-4269-A5EF-6E00C687C157}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="32">
   <si>
     <t>Name</t>
   </si>
@@ -72,18 +72,9 @@
     <t>Id</t>
   </si>
   <si>
-    <t>ÁNGULOS</t>
-  </si>
-  <si>
     <t>Tipo</t>
   </si>
   <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>I</t>
-  </si>
-  <si>
     <t>X</t>
   </si>
   <si>
@@ -96,9 +87,6 @@
     <t>12,14,16</t>
   </si>
   <si>
-    <t>6 , 8,10</t>
-  </si>
-  <si>
     <t>7,9,11</t>
   </si>
   <si>
@@ -118,6 +106,21 @@
   </si>
   <si>
     <t>POSIBLES ANGULOS A EXTRAER</t>
+  </si>
+  <si>
+    <t>6,8,10</t>
+  </si>
+  <si>
+    <t>Articulaciones</t>
+  </si>
+  <si>
+    <t>Lado</t>
+  </si>
+  <si>
+    <t>Derecha</t>
+  </si>
+  <si>
+    <t>Izquierda</t>
   </si>
 </sst>
 </file>
@@ -521,7 +524,7 @@
   <dimension ref="B2:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:C17"/>
+      <selection activeCell="D29" sqref="B23:D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,10 +541,10 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
@@ -682,81 +685,84 @@
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>15</v>
+      </c>
       <c r="C23" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="D23" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D24" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C25" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D25" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D26" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C27" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D27" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C28" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D28" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C29" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D29" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>